<commit_message>
Submit TST1149 ,TST547 ,TST548 ,TST580 ,TST832
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/Keywordscripts/TST592_DeleteAnActionSetWithUsersRight.xlsx
+++ b/NformTester/NformTester/Keywordscripts/TST592_DeleteAnActionSetWithUsersRight.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="15480" windowHeight="9570"/>
@@ -3952,7 +3952,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3960,27 +3960,27 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3988,7 +3988,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -4178,7 +4178,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="1"/>
     <cellStyle name="常规 2 2" xfId="2"/>
   </cellStyles>
@@ -4203,7 +4203,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4489,24 +4489,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.75" style="16" customWidth="1"/>
-    <col min="2" max="2" width="28.375" style="16" customWidth="1"/>
-    <col min="5" max="5" width="29.75" customWidth="1"/>
-    <col min="6" max="6" width="29.25" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" style="16" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="34.125" customWidth="1"/>
-    <col min="9" max="9" width="31.875" customWidth="1"/>
-    <col min="11" max="11" width="10.125" customWidth="1"/>
-    <col min="12" max="12" width="13.75" customWidth="1"/>
+    <col min="8" max="8" width="34.140625" customWidth="1"/>
+    <col min="9" max="9" width="31.85546875" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" ht="25.5">
       <c r="A1" s="1" t="s">
         <v>818</v>
       </c>
@@ -4550,7 +4550,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15">
+    <row r="2" spans="1:15">
       <c r="A2" s="2" t="s">
         <v>820</v>
       </c>
@@ -4636,7 +4636,7 @@
       <c r="M4" s="3"/>
       <c r="N4" s="15"/>
     </row>
-    <row r="5" spans="1:15" ht="15">
+    <row r="5" spans="1:15">
       <c r="A5" s="2" t="s">
         <v>826</v>
       </c>
@@ -4870,7 +4870,7 @@
       <c r="N12" s="19"/>
       <c r="O12" s="17"/>
     </row>
-    <row r="13" spans="1:15" s="16" customFormat="1" ht="15">
+    <row r="13" spans="1:15" s="16" customFormat="1">
       <c r="A13" s="2"/>
       <c r="B13" s="11"/>
       <c r="C13" s="3">
@@ -5162,7 +5162,7 @@
       <c r="N22" s="19"/>
       <c r="O22" s="17"/>
     </row>
-    <row r="23" spans="1:15" ht="15">
+    <row r="23" spans="1:15">
       <c r="A23" s="22" t="s">
         <v>815</v>
       </c>
@@ -5570,7 +5570,7 @@
       <c r="M38" s="3"/>
       <c r="N38" s="15"/>
     </row>
-    <row r="39" spans="3:14" ht="15">
+    <row r="39" spans="3:14">
       <c r="C39" s="3">
         <v>38</v>
       </c>
@@ -5870,7 +5870,7 @@
       <c r="M50" s="3"/>
       <c r="N50" s="15"/>
     </row>
-    <row r="51" spans="3:14" s="16" customFormat="1" ht="15">
+    <row r="51" spans="3:14" s="16" customFormat="1">
       <c r="C51" s="3">
         <v>50</v>
       </c>
@@ -6378,7 +6378,7 @@
       <c r="M74" s="3"/>
       <c r="N74" s="15"/>
     </row>
-    <row r="75" spans="3:14" ht="15">
+    <row r="75" spans="3:14">
       <c r="C75" s="3"/>
       <c r="D75" s="14"/>
       <c r="E75" s="3"/>
@@ -6511,7 +6511,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:85">
       <c r="A1" t="s">
@@ -10420,7 +10420,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1066">
       <c r="A1" t="s">
@@ -29480,10 +29480,10 @@
       <selection activeCell="F91" sqref="F91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.75" customWidth="1"/>
-    <col min="2" max="2" width="28.375" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>